<commit_message>
Added analysis of decoder to report
</commit_message>
<xml_diff>
--- a/analysis.xlsx
+++ b/analysis.xlsx
@@ -1,36 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robbie/huffman/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Robbie\Documents\dev\huffman\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="980" yWindow="460" windowWidth="27820" windowHeight="17540" xr2:uid="{B680642F-3900-4156-BD98-AD1C67CCCD87}"/>
+    <workbookView xWindow="975" yWindow="465" windowWidth="27825" windowHeight="17535" activeTab="1" xr2:uid="{B680642F-3900-4156-BD98-AD1C67CCCD87}"/>
   </bookViews>
   <sheets>
-    <sheet name="file size against time" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="file size against decode time" sheetId="5" r:id="rId1"/>
+    <sheet name="file size against encode time" sheetId="2" r:id="rId2"/>
+    <sheet name="DATA" sheetId="1" r:id="rId3"/>
+    <sheet name="file size against time backup" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet1 backup" sheetId="3" r:id="rId5"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$F$3:$F$10</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$H$3:$H$10</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">Sheet1!$F$3:$F$10</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">Sheet1!$H$3:$H$10</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$F$3:$F$10</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!$H$3:$H$10</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$F$3:$F$10</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$H$3:$H$10</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Sheet1!$F$3:$F$10</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Sheet1!$H$3:$H$10</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">Sheet1!$F$3:$F$10</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">Sheet1!$H$3:$H$10</definedName>
-    <definedName name="_xlchart.v2.10" hidden="1">Sheet1!$F$3:$F$10</definedName>
-    <definedName name="_xlchart.v2.11" hidden="1">Sheet1!$H$3:$H$10</definedName>
-  </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -41,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="24">
   <si>
     <t>Item</t>
   </si>
@@ -89,6 +76,30 @@
   </si>
   <si>
     <t>compression ratio</t>
+  </si>
+  <si>
+    <t>t_0 m</t>
+  </si>
+  <si>
+    <t>t_1 m</t>
+  </si>
+  <si>
+    <t>t_2 m</t>
+  </si>
+  <si>
+    <t>avg m</t>
+  </si>
+  <si>
+    <t>t_0 m d</t>
+  </si>
+  <si>
+    <t>t_1 m d</t>
+  </si>
+  <si>
+    <t>t_2 m d</t>
+  </si>
+  <si>
+    <t>avg m d</t>
   </si>
 </sst>
 </file>
@@ -163,6 +174,494 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="108"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="8"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Segoe UI Symbol" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
+                <a:ea typeface="Segoe UI Symbol" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="2400" b="0">
+                <a:latin typeface="Segoe UI Symbol" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
+                <a:ea typeface="Segoe UI Symbol" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
+                <a:cs typeface="Segoe UI Historic" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
+              </a:rPr>
+              <a:t>File Size against Decoding Time</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="2400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Segoe UI Symbol" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
+              <a:ea typeface="Segoe UI Symbol" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="50800" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="73B7FA"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent6">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent6">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent6">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="101600" cap="rnd">
+                <a:solidFill>
+                  <a:srgbClr val="73B7FA"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>DATA!$R$3:$R$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>716</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5250</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>57024</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>61824</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>462070</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>927207</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1055021</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2668114</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>DATA!$P$3:$P$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1.0026666666666668E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.3456666666666673E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.58448666666666671</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.53110999999999997</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.3585233333333329</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.8081466666666666</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.5954100000000002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>15.972369999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-97AC-4170-ABC4-AF78D32A853E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1355249376"/>
+        <c:axId val="1355251072"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1355249376"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1600"/>
+                  <a:t>File Size (bytes)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="#,##0" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1355251072"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1355251072"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1600"/>
+                  <a:t>Decoding Time (s)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Segoe UI Symbol" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
+                <a:ea typeface="Segoe UI Symbol" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1355249376"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -306,7 +805,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$H$3:$H$10</c:f>
+              <c:f>DATA!$R$3:$R$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -339,33 +838,33 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$F$3:$F$10</c:f>
+              <c:f>DATA!$K$3:$K$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>4.2766666666666665E-3</c:v>
+                  <c:v>5.5633333333333333E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.3899999999999999E-3</c:v>
+                  <c:v>1.052E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.8196666666666665E-2</c:v>
+                  <c:v>3.4236666666666665E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.0380000000000001E-2</c:v>
+                  <c:v>6.7493333333333336E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.32449333333333336</c:v>
+                  <c:v>0.23818666666666669</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.70046666666666668</c:v>
+                  <c:v>0.51472333333333331</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.76849333333333336</c:v>
+                  <c:v>0.54151000000000005</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.9577600000000002</c:v>
+                  <c:v>1.4072366666666667</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -650,7 +1149,507 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="108"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="8"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Segoe UI Symbol" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
+                <a:ea typeface="Segoe UI Symbol" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="2400" b="0">
+                <a:latin typeface="Segoe UI Symbol" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
+                <a:ea typeface="Segoe UI Symbol" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
+                <a:cs typeface="Segoe UI Historic" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
+              </a:rPr>
+              <a:t>File Size against Encoding Time</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="2400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Segoe UI Symbol" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
+              <a:ea typeface="Segoe UI Symbol" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="50800" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="73B7FA"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:gradFill rotWithShape="1">
+                <a:gsLst>
+                  <a:gs pos="0">
+                    <a:schemeClr val="accent6">
+                      <a:satMod val="103000"/>
+                      <a:lumMod val="102000"/>
+                      <a:tint val="94000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="50000">
+                    <a:schemeClr val="accent6">
+                      <a:satMod val="110000"/>
+                      <a:lumMod val="100000"/>
+                      <a:shade val="100000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                  <a:gs pos="100000">
+                    <a:schemeClr val="accent6">
+                      <a:lumMod val="99000"/>
+                      <a:satMod val="120000"/>
+                      <a:shade val="78000"/>
+                    </a:schemeClr>
+                  </a:gs>
+                </a:gsLst>
+                <a:lin ang="5400000" scaled="0"/>
+              </a:gradFill>
+              <a:ln w="101600" cap="rnd">
+                <a:solidFill>
+                  <a:srgbClr val="73B7FA"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst>
+                <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="000000">
+                    <a:alpha val="63000"/>
+                  </a:srgbClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>DATA!$R$3:$R$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>716</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5250</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>57024</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>61824</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>462070</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>927207</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1055021</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2668114</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>DATA!$F$3:$F$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>4.2766666666666665E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.3899999999999999E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.8196666666666665E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.0380000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.32449333333333336</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.70046666666666668</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.76849333333333336</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.9577600000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B68C-40AB-A49D-9059182B8945}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1355249376"/>
+        <c:axId val="1355251072"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1355249376"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1600"/>
+                  <a:t>File Size (bytes)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="#,##0" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1355251072"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1355251072"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1600"/>
+                  <a:t>Encoding Time (s)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Segoe UI Symbol" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
+                <a:ea typeface="Segoe UI Symbol" panose="020B0502040204020203" pitchFamily="34" charset="0"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1355249376"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinear" id="19">
+  <a:schemeClr val="accent6"/>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinear" id="19">
+  <a:schemeClr val="accent6"/>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="withinLinear" id="19">
   <a:schemeClr val="accent6"/>
 </cs:colorStyle>
@@ -1158,11 +2157,1037 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="343">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="343">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx2"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{EF03636C-2D11-4839-9B90-964BA8EDD5E7}">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="178" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{B8DAF98C-FB19-B847-9F98-134E4E7C1335}">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="139" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="178" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{9B8CE9FA-F3A1-48BD-B154-C4079D0D9EDF}">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="178" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1173,13 +3198,79 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9317290" cy="6077009"/>
+    <xdr:ext cx="9308171" cy="6078963"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7798BC86-335E-4DDC-9529-86813F8956E0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="9308171" cy="6078963"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F3E2EEB1-3D61-C345-9DAE-5C44EBEE6764}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="9308171" cy="6078963"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{08395DAD-80A9-47A3-BC38-BDD35470C7BB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1499,19 +3590,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DD27AFA-EFC3-4E88-A9B2-E94EC2144EA1}">
-  <dimension ref="B2:M12"/>
+  <dimension ref="B2:W12"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="150" workbookViewId="0">
-      <selection activeCell="F3" activeCellId="1" sqref="H3:H10 F3:F10"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:W10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.6640625" customWidth="1"/>
-    <col min="9" max="9" width="20.33203125" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" customWidth="1"/>
+    <col min="14" max="14" width="20.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -1528,16 +3619,538 @@
         <v>12</v>
       </c>
       <c r="H2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M2" t="s">
+        <v>20</v>
+      </c>
+      <c r="N2" t="s">
+        <v>21</v>
+      </c>
+      <c r="O2" t="s">
+        <v>22</v>
+      </c>
+      <c r="P2" t="s">
+        <v>23</v>
+      </c>
+      <c r="R2" t="s">
         <v>13</v>
       </c>
+      <c r="T2" t="s">
+        <v>14</v>
+      </c>
+      <c r="W2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>4.3499999999999997E-3</v>
+      </c>
+      <c r="D3">
+        <v>4.3400000000000001E-3</v>
+      </c>
+      <c r="E3">
+        <v>4.1399999999999996E-3</v>
+      </c>
+      <c r="F3">
+        <f>AVERAGE(C3:E3)</f>
+        <v>4.2766666666666665E-3</v>
+      </c>
+      <c r="H3">
+        <v>5.47E-3</v>
+      </c>
+      <c r="I3">
+        <v>4.8700000000000002E-3</v>
+      </c>
+      <c r="J3">
+        <v>6.3499999999999997E-3</v>
+      </c>
+      <c r="K3">
+        <f>AVERAGE(H3:J3)</f>
+        <v>5.5633333333333333E-3</v>
+      </c>
+      <c r="M3">
+        <v>1.072E-2</v>
+      </c>
+      <c r="N3">
+        <v>9.6600000000000002E-3</v>
+      </c>
+      <c r="O3">
+        <v>9.7000000000000003E-3</v>
+      </c>
+      <c r="P3">
+        <f>AVERAGE(M3:O3)</f>
+        <v>1.0026666666666668E-2</v>
+      </c>
+      <c r="R3">
+        <v>716</v>
+      </c>
+      <c r="T3">
+        <v>451</v>
+      </c>
+      <c r="W3" s="1">
+        <f>T3/R3</f>
+        <v>0.62988826815642462</v>
+      </c>
+    </row>
+    <row r="4" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>7.2500000000000004E-3</v>
+      </c>
+      <c r="D4">
+        <v>7.3200000000000001E-3</v>
+      </c>
+      <c r="E4">
+        <v>7.6E-3</v>
+      </c>
+      <c r="F4">
+        <f>AVERAGE(C4:E4)</f>
+        <v>7.3899999999999999E-3</v>
+      </c>
+      <c r="H4">
+        <v>1.0840000000000001E-2</v>
+      </c>
+      <c r="I4">
+        <v>9.8899999999999995E-3</v>
+      </c>
+      <c r="J4">
+        <v>1.0829999999999999E-2</v>
+      </c>
+      <c r="K4">
+        <f>AVERAGE(H4:J4)</f>
+        <v>1.052E-2</v>
+      </c>
+      <c r="M4">
+        <v>5.3670000000000002E-2</v>
+      </c>
+      <c r="N4">
+        <v>5.5640000000000002E-2</v>
+      </c>
+      <c r="O4">
+        <v>5.1060000000000001E-2</v>
+      </c>
+      <c r="P4">
+        <f>AVERAGE(M4:O4)</f>
+        <v>5.3456666666666673E-2</v>
+      </c>
+      <c r="R4">
+        <v>5250</v>
+      </c>
+      <c r="T4">
+        <v>2904</v>
+      </c>
+      <c r="W4" s="1">
+        <f>T4/R4</f>
+        <v>0.55314285714285716</v>
+      </c>
+    </row>
+    <row r="5" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5">
+        <v>4.8899999999999999E-2</v>
+      </c>
+      <c r="D5">
+        <v>4.7840000000000001E-2</v>
+      </c>
+      <c r="E5">
+        <v>4.7849999999999997E-2</v>
+      </c>
+      <c r="F5">
+        <f>AVERAGE(C5:E5)</f>
+        <v>4.8196666666666665E-2</v>
+      </c>
+      <c r="H5">
+        <v>3.431E-2</v>
+      </c>
+      <c r="I5">
+        <v>3.3919999999999999E-2</v>
+      </c>
+      <c r="J5">
+        <v>3.4479999999999997E-2</v>
+      </c>
+      <c r="K5">
+        <f>AVERAGE(H5:J5)</f>
+        <v>3.4236666666666665E-2</v>
+      </c>
+      <c r="M5">
+        <v>0.58875999999999995</v>
+      </c>
+      <c r="N5">
+        <v>0.58401999999999998</v>
+      </c>
+      <c r="O5">
+        <v>0.58067999999999997</v>
+      </c>
+      <c r="P5">
+        <f>AVERAGE(M5:O5)</f>
+        <v>0.58448666666666671</v>
+      </c>
+      <c r="R5">
+        <v>57024</v>
+      </c>
+      <c r="T5">
+        <v>35132</v>
+      </c>
+      <c r="W5" s="1">
+        <f>T5/R5</f>
+        <v>0.61609147025813693</v>
+      </c>
+    </row>
+    <row r="6" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="D6">
+        <v>4.827E-2</v>
+      </c>
+      <c r="E6">
+        <v>4.8869999999999997E-2</v>
+      </c>
+      <c r="F6">
+        <f>AVERAGE(C6:E6)</f>
+        <v>5.0380000000000001E-2</v>
+      </c>
+      <c r="H6">
+        <v>6.7699999999999996E-2</v>
+      </c>
+      <c r="I6">
+        <v>6.5729999999999997E-2</v>
+      </c>
+      <c r="J6">
+        <v>6.905E-2</v>
+      </c>
+      <c r="K6">
+        <f>AVERAGE(H6:J6)</f>
+        <v>6.7493333333333336E-2</v>
+      </c>
+      <c r="M6">
+        <v>0.56147000000000002</v>
+      </c>
+      <c r="N6">
+        <v>0.47095999999999999</v>
+      </c>
+      <c r="O6">
+        <v>0.56089999999999995</v>
+      </c>
+      <c r="P6">
+        <f>AVERAGE(M6:O6)</f>
+        <v>0.53110999999999997</v>
+      </c>
+      <c r="R6">
+        <v>61824</v>
+      </c>
+      <c r="T6">
+        <v>33235</v>
+      </c>
+      <c r="W6" s="1">
+        <f>T6/R6</f>
+        <v>0.53757440476190477</v>
+      </c>
+    </row>
+    <row r="7" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7">
+        <v>0.33424999999999999</v>
+      </c>
+      <c r="D7">
+        <v>0.30703000000000003</v>
+      </c>
+      <c r="E7">
+        <v>0.3322</v>
+      </c>
+      <c r="F7">
+        <f>AVERAGE(C7:E7)</f>
+        <v>0.32449333333333336</v>
+      </c>
+      <c r="H7">
+        <v>0.23680999999999999</v>
+      </c>
+      <c r="I7">
+        <v>0.23952000000000001</v>
+      </c>
+      <c r="J7">
+        <v>0.23823</v>
+      </c>
+      <c r="K7">
+        <f>AVERAGE(H7:J7)</f>
+        <v>0.23818666666666669</v>
+      </c>
+      <c r="M7">
+        <v>3.2929599999999999</v>
+      </c>
+      <c r="N7">
+        <v>2.9597600000000002</v>
+      </c>
+      <c r="O7">
+        <v>3.8228499999999999</v>
+      </c>
+      <c r="P7">
+        <f>AVERAGE(M7:O7)</f>
+        <v>3.3585233333333329</v>
+      </c>
+      <c r="R7">
+        <v>462070</v>
+      </c>
+      <c r="T7">
+        <v>264179</v>
+      </c>
+      <c r="W7" s="1">
+        <f>T7/R7</f>
+        <v>0.57172939165061576</v>
+      </c>
+    </row>
+    <row r="8" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8">
+        <v>0.74341999999999997</v>
+      </c>
+      <c r="D8">
+        <v>0.65576000000000001</v>
+      </c>
+      <c r="E8">
+        <v>0.70221999999999996</v>
+      </c>
+      <c r="F8">
+        <f>AVERAGE(C8:E8)</f>
+        <v>0.70046666666666668</v>
+      </c>
+      <c r="H8">
+        <v>0.51712999999999998</v>
+      </c>
+      <c r="I8">
+        <v>0.49049999999999999</v>
+      </c>
+      <c r="J8">
+        <v>0.53654000000000002</v>
+      </c>
+      <c r="K8">
+        <f>AVERAGE(H8:J8)</f>
+        <v>0.51472333333333331</v>
+      </c>
+      <c r="M8">
+        <v>5.9124699999999999</v>
+      </c>
+      <c r="N8">
+        <v>6.3533900000000001</v>
+      </c>
+      <c r="O8">
+        <v>5.1585799999999997</v>
+      </c>
+      <c r="P8">
+        <f>AVERAGE(M8:O8)</f>
+        <v>5.8081466666666666</v>
+      </c>
+      <c r="R8">
+        <v>927207</v>
+      </c>
+      <c r="T8">
+        <v>518531</v>
+      </c>
+      <c r="W8" s="1">
+        <f>T8/R8</f>
+        <v>0.55923973826772233</v>
+      </c>
+    </row>
+    <row r="9" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>0.76829000000000003</v>
+      </c>
+      <c r="D9">
+        <v>0.77971999999999997</v>
+      </c>
+      <c r="E9">
+        <v>0.75746999999999998</v>
+      </c>
+      <c r="F9">
+        <f>AVERAGE(C9:E9)</f>
+        <v>0.76849333333333336</v>
+      </c>
+      <c r="H9">
+        <v>0.54171000000000002</v>
+      </c>
+      <c r="I9">
+        <v>0.54288999999999998</v>
+      </c>
+      <c r="J9">
+        <v>0.53993000000000002</v>
+      </c>
+      <c r="K9">
+        <f>AVERAGE(H9:J9)</f>
+        <v>0.54151000000000005</v>
+      </c>
+      <c r="M9">
+        <v>7.3129499999999998</v>
+      </c>
+      <c r="N9">
+        <v>6.2022000000000004</v>
+      </c>
+      <c r="O9">
+        <v>6.2710800000000004</v>
+      </c>
+      <c r="P9">
+        <f>AVERAGE(M9:O9)</f>
+        <v>6.5954100000000002</v>
+      </c>
+      <c r="R9">
+        <v>1055021</v>
+      </c>
+      <c r="T9">
+        <v>614807</v>
+      </c>
+      <c r="W9" s="1">
+        <f>T9/R9</f>
+        <v>0.58274385059633882</v>
+      </c>
+    </row>
+    <row r="10" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10">
+        <v>2.0781700000000001</v>
+      </c>
+      <c r="D10">
+        <v>1.88652</v>
+      </c>
+      <c r="E10">
+        <v>1.90859</v>
+      </c>
+      <c r="F10">
+        <f>AVERAGE(C10:E10)</f>
+        <v>1.9577600000000002</v>
+      </c>
+      <c r="H10">
+        <v>1.3998699999999999</v>
+      </c>
+      <c r="I10">
+        <v>1.4307099999999999</v>
+      </c>
+      <c r="J10">
+        <v>1.39113</v>
+      </c>
+      <c r="K10">
+        <f>AVERAGE(H10:J10)</f>
+        <v>1.4072366666666667</v>
+      </c>
+      <c r="M10">
+        <v>15.858919999999999</v>
+      </c>
+      <c r="N10">
+        <v>16.606369999999998</v>
+      </c>
+      <c r="O10">
+        <v>15.45182</v>
+      </c>
+      <c r="P10">
+        <f>AVERAGE(M10:O10)</f>
+        <v>15.972369999999998</v>
+      </c>
+      <c r="R10">
+        <v>2668114</v>
+      </c>
+      <c r="T10">
+        <v>1560590</v>
+      </c>
+      <c r="W10" s="1">
+        <f>T10/R10</f>
+        <v>0.58490379346609622</v>
+      </c>
+    </row>
+    <row r="12" spans="2:23" x14ac:dyDescent="0.25">
+      <c r="W12" s="2">
+        <f>AVERAGE(W3:W11)</f>
+        <v>0.57941422178751201</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="B3:W10">
+    <sortCondition ref="R3:R10"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C3A6BED-3BCF-4DF6-BE56-23330F697571}">
+  <dimension ref="B2:R12"/>
+  <sheetViews>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:R10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="13.7109375" customWidth="1"/>
+    <col min="14" max="14" width="20.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" t="s">
+        <v>17</v>
+      </c>
       <c r="J2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" t="s">
+        <v>19</v>
+      </c>
+      <c r="M2" t="s">
+        <v>13</v>
+      </c>
+      <c r="O2" t="s">
         <v>14</v>
       </c>
-      <c r="M2" t="s">
+      <c r="R2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>1</v>
       </c>
@@ -1554,18 +4167,18 @@
         <f t="shared" ref="F3:F10" si="0">AVERAGE(C3:E3)</f>
         <v>4.2766666666666665E-3</v>
       </c>
-      <c r="H3">
+      <c r="M3">
         <v>716</v>
       </c>
-      <c r="J3">
+      <c r="O3">
         <v>451</v>
       </c>
-      <c r="M3" s="1">
-        <f t="shared" ref="M3:M10" si="1">J3/H3</f>
+      <c r="R3" s="1">
+        <f t="shared" ref="R3:R10" si="1">O3/M3</f>
         <v>0.62988826815642462</v>
       </c>
     </row>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>2</v>
       </c>
@@ -1582,18 +4195,18 @@
         <f t="shared" si="0"/>
         <v>7.3899999999999999E-3</v>
       </c>
-      <c r="H4">
+      <c r="M4">
         <v>5250</v>
       </c>
-      <c r="J4">
+      <c r="O4">
         <v>2904</v>
       </c>
-      <c r="M4" s="1">
+      <c r="R4" s="1">
         <f t="shared" si="1"/>
         <v>0.55314285714285716</v>
       </c>
     </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>5</v>
       </c>
@@ -1610,18 +4223,18 @@
         <f t="shared" si="0"/>
         <v>4.8196666666666665E-2</v>
       </c>
-      <c r="H5">
+      <c r="M5">
         <v>57024</v>
       </c>
-      <c r="J5">
+      <c r="O5">
         <v>35132</v>
       </c>
-      <c r="M5" s="1">
+      <c r="R5" s="1">
         <f t="shared" si="1"/>
         <v>0.61609147025813693</v>
       </c>
     </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>3</v>
       </c>
@@ -1638,18 +4251,18 @@
         <f t="shared" si="0"/>
         <v>5.0380000000000001E-2</v>
       </c>
-      <c r="H6">
+      <c r="M6">
         <v>61824</v>
       </c>
-      <c r="J6">
+      <c r="O6">
         <v>33235</v>
       </c>
-      <c r="M6" s="1">
+      <c r="R6" s="1">
         <f t="shared" si="1"/>
         <v>0.53757440476190477</v>
       </c>
     </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>7</v>
       </c>
@@ -1666,18 +4279,18 @@
         <f t="shared" si="0"/>
         <v>0.32449333333333336</v>
       </c>
-      <c r="H7">
+      <c r="M7">
         <v>462070</v>
       </c>
-      <c r="J7">
+      <c r="O7">
         <v>264179</v>
       </c>
-      <c r="M7" s="1">
+      <c r="R7" s="1">
         <f t="shared" si="1"/>
         <v>0.57172939165061576</v>
       </c>
     </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>4</v>
       </c>
@@ -1694,18 +4307,18 @@
         <f t="shared" si="0"/>
         <v>0.70046666666666668</v>
       </c>
-      <c r="H8">
+      <c r="M8">
         <v>927207</v>
       </c>
-      <c r="J8">
+      <c r="O8">
         <v>518531</v>
       </c>
-      <c r="M8" s="1">
+      <c r="R8" s="1">
         <f t="shared" si="1"/>
         <v>0.55923973826772233</v>
       </c>
     </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>8</v>
       </c>
@@ -1722,18 +4335,18 @@
         <f t="shared" si="0"/>
         <v>0.76849333333333336</v>
       </c>
-      <c r="H9">
+      <c r="M9">
         <v>1055021</v>
       </c>
-      <c r="J9">
+      <c r="O9">
         <v>614807</v>
       </c>
-      <c r="M9" s="1">
+      <c r="R9" s="1">
         <f t="shared" si="1"/>
         <v>0.58274385059633882</v>
       </c>
     </row>
-    <row r="10" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
         <v>6</v>
       </c>
@@ -1750,27 +4363,24 @@
         <f t="shared" si="0"/>
         <v>1.9577600000000002</v>
       </c>
-      <c r="H10">
+      <c r="M10">
         <v>2668114</v>
       </c>
-      <c r="J10">
+      <c r="O10">
         <v>1560590</v>
       </c>
-      <c r="M10" s="1">
+      <c r="R10" s="1">
         <f t="shared" si="1"/>
         <v>0.58490379346609622</v>
       </c>
     </row>
-    <row r="12" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="M12" s="2">
-        <f>AVERAGE(M3:M11)</f>
+    <row r="12" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="R12" s="2">
+        <f>AVERAGE(R3:R11)</f>
         <v>0.57941422178751201</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="B3:M10">
-    <sortCondition ref="H3:H10"/>
-  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>